<commit_message>
13:11 - 11.02.2025 - Monday with TIll polish
</commit_message>
<xml_diff>
--- a/NachDurchlaufplan/excelFiles/1-H&S&C.xlsx
+++ b/NachDurchlaufplan/excelFiles/1-H&S&C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/pit5lo_bosch_com/Documents/Ausbildung - Fachinformatik/NachDurchlaufplan/excelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="345" documentId="13_ncr:1_{4450C31E-C781-4AF7-8D18-6AAE55A9B24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBB48362-D8BB-4723-BA34-9C249C9A9DC9}"/>
+  <xr:revisionPtr revIDLastSave="357" documentId="13_ncr:1_{4450C31E-C781-4AF7-8D18-6AAE55A9B24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BC92435-3AB6-4BD3-98D1-0DC58C35543E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
+    <workbookView minimized="1" xWindow="30210" yWindow="1395" windowWidth="17250" windowHeight="8910" activeTab="4" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
   </bookViews>
   <sheets>
     <sheet name="Montag" sheetId="1" r:id="rId1"/>
@@ -1227,6 +1227,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1251,40 +1287,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1308,31 +1317,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1687,20 +1687,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8125109F-5B4D-4D92-87E5-6766938EA6FC}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C28"/>
+    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1714,11 +1714,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="64" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -1726,61 +1726,61 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="54"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="37" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
         <v>0.375</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="62" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="51"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="63"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="64" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="35" t="s">
@@ -1788,61 +1788,61 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="25">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="54"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="54"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="54"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="53"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="37" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="60" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="41" t="s">
@@ -1850,69 +1850,69 @@
       </c>
       <c r="D14" s="28"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="68"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="68"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="69"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="61">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="53">
         <v>0.5</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-    </row>
-    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="54"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="54"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="55"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+    </row>
+    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="56" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="35" t="s">
@@ -1920,87 +1920,87 @@
       </c>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="65"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="65"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="66"/>
+      <c r="B25" s="58"/>
       <c r="C25" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="56" t="s">
         <v>80</v>
       </c>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="65"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="57"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="57"/>
-      <c r="C28" s="66"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="58"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="25">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B18:D21"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2011,20 +2011,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A2A2E4-2443-47D7-9D3C-2ED84D5A5B04}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="70.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="70.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2038,55 +2038,55 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="62" t="s">
         <v>75</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="78"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="78"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="78"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="29">
         <v>0.375</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="26"/>
     </row>
-    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="64" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="35" t="s">
@@ -2094,21 +2094,21 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="53"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="37" t="s">
         <v>76</v>
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="64" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="35" t="s">
@@ -2116,21 +2116,21 @@
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="53"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="37" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="64" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="35" t="s">
@@ -2138,41 +2138,41 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="53"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="37" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="62" t="s">
         <v>78</v>
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="51"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="63"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="64" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="35" t="s">
@@ -2180,17 +2180,17 @@
       </c>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="53"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="37" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29">
         <v>0.48958333333333298</v>
       </c>
@@ -2202,39 +2202,39 @@
       </c>
       <c r="D17" s="23"/>
     </row>
-    <row r="18" spans="1:4" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70">
+    <row r="18" spans="1:4" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="73">
         <v>0.5</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="76"/>
-    </row>
-    <row r="19" spans="1:4" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="76"/>
-    </row>
-    <row r="20" spans="1:4" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="76"/>
-    </row>
-    <row r="21" spans="1:4" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="72"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="76"/>
-    </row>
-    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="59"/>
+      <c r="D18" s="79"/>
+    </row>
+    <row r="19" spans="1:4" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="74"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="79"/>
+    </row>
+    <row r="20" spans="1:4" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="74"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="79"/>
+    </row>
+    <row r="21" spans="1:4" ht="9.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="75"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="79"/>
+    </row>
+    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="64" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="35" t="s">
@@ -2242,72 +2242,77 @@
       </c>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="78" t="s">
+      <c r="B23" s="66"/>
+      <c r="C23" s="71" t="s">
         <v>82</v>
       </c>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="54"/>
-      <c r="C24" s="78"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="71"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="78" t="s">
+      <c r="B25" s="66"/>
+      <c r="C25" s="71" t="s">
         <v>83</v>
       </c>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="78"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="71"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="78" t="s">
+      <c r="B27" s="66"/>
+      <c r="C27" s="71" t="s">
         <v>84</v>
       </c>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="29">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="51"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B18:D21"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="B13:B14"/>
@@ -2318,11 +2323,6 @@
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B18:D21"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2333,20 +2333,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317F4A4C-3A30-4CB8-B02B-BC300C6A4A83}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C28"/>
+    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2360,65 +2360,65 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="56" t="s">
         <v>85</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="65"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="57"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="65"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="65"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>0.375</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="56"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="36" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="67" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="35" t="s">
@@ -2426,57 +2426,57 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="56"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="56"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="56"/>
+      <c r="B11" s="68"/>
       <c r="C11" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="56"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="57"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="37" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>0.45833333333333298</v>
       </c>
@@ -2488,15 +2488,15 @@
       </c>
       <c r="D14" s="34"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="73"/>
-      <c r="C15" s="74"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="77"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19">
         <v>0.47916666666666702</v>
       </c>
@@ -2508,7 +2508,7 @@
       </c>
       <c r="D16" s="23"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>0.48958333333333298</v>
       </c>
@@ -2520,107 +2520,107 @@
       </c>
       <c r="D17" s="30"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="73">
         <v>0.5</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="76"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="76"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="76"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="72"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="76"/>
-    </row>
-    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="59"/>
+      <c r="D18" s="79"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="74"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="79"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="74"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="79"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="75"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="79"/>
+    </row>
+    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="62" t="s">
         <v>88</v>
       </c>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="78"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="54"/>
-      <c r="C24" s="78" t="s">
+      <c r="B24" s="66"/>
+      <c r="C24" s="71" t="s">
         <v>87</v>
       </c>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="78"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="71"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="78" t="s">
+      <c r="B26" s="66"/>
+      <c r="C26" s="71" t="s">
         <v>86</v>
       </c>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="78"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="71"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="29">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="51"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2647,19 +2647,19 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B27" sqref="B27:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2673,11 +2673,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="64" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -2685,21 +2685,21 @@
       </c>
       <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="37" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="64" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="35" t="s">
@@ -2707,21 +2707,21 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="37" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>0.375</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="64" t="s">
         <v>61</v>
       </c>
       <c r="C6" s="35" t="s">
@@ -2729,21 +2729,21 @@
       </c>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="77"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="36" t="s">
         <v>59</v>
       </c>
       <c r="D7" s="26"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="64" t="s">
         <v>62</v>
       </c>
       <c r="C8" s="35" t="s">
@@ -2751,49 +2751,49 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="78" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="71" t="s">
         <v>63</v>
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="78"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="54"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="53"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="37" t="s">
         <v>66</v>
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="64" t="s">
         <v>65</v>
       </c>
       <c r="C13" s="35" t="s">
@@ -2801,121 +2801,121 @@
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="77"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="42" t="s">
         <v>68</v>
       </c>
       <c r="D14" s="26"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="62" t="s">
         <v>98</v>
       </c>
       <c r="D15" s="27"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="78"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="51"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="73">
         <v>0.5</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="76"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="76"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="76"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="72"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="76"/>
-    </row>
-    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="59"/>
+      <c r="D18" s="79"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="74"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="79"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="74"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="79"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="75"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="79"/>
+    </row>
+    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="56" t="s">
         <v>99</v>
       </c>
       <c r="D22" s="27"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="78"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="57"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="54"/>
-      <c r="C24" s="78"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="57"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="78"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="57"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="29">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="51"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="68" t="s">
         <v>89</v>
       </c>
       <c r="C27" s="41" t="s">
@@ -2923,28 +2923,34 @@
       </c>
       <c r="D27" s="28"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="29">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="57"/>
+      <c r="B28" s="69"/>
       <c r="C28" s="37" t="s">
         <v>91</v>
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B8:B12"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A18:A21"/>
@@ -2953,12 +2959,6 @@
     <mergeCell ref="B22:B26"/>
     <mergeCell ref="C22:C26"/>
     <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B8:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2968,20 +2968,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42D2DE4-CD58-4047-AD59-C2BB7A83B7F8}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C17"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2995,247 +2995,247 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43">
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="83"/>
+      <c r="C2" s="82"/>
       <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="68"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="60"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="29">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="48"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="62" t="s">
         <v>92</v>
       </c>
       <c r="D5" s="27"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>0.375</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="78"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="78"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="78"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="78"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="78"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="78"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="78"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="29">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="51"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="63"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="65" t="s">
+      <c r="C14" s="57" t="s">
         <v>94</v>
       </c>
       <c r="D14" s="49"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="65"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="66"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="73">
         <v>0.5</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="76"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="76"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="76"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="72"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="76"/>
-    </row>
-    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="59"/>
+      <c r="D18" s="79"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="74"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="79"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="74"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="79"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="75"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="79"/>
+    </row>
+    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="62" t="s">
         <v>95</v>
       </c>
       <c r="D22" s="27"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="29">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="51"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="63"/>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="82" t="s">
+      <c r="B24" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="85" t="s">
+      <c r="C24" s="84" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="28"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="78"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="71"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="78" t="s">
+      <c r="B26" s="66"/>
+      <c r="C26" s="71" t="s">
         <v>73</v>
       </c>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="78"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="71"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="29">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="51"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -3261,20 +3261,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E2BF86-5BDF-480D-A26D-C21A6EA25768}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>0.33333333333333331</v>
       </c>
@@ -3296,7 +3296,7 @@
       <c r="C2" s="12"/>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>0.34375</v>
       </c>
@@ -3304,7 +3304,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>0.35416666666666702</v>
       </c>
@@ -3312,7 +3312,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>0.36458333333333298</v>
       </c>
@@ -3320,7 +3320,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>0.375</v>
       </c>
@@ -3328,7 +3328,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>0.38541666666666702</v>
       </c>
@@ -3336,7 +3336,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>0.39583333333333298</v>
       </c>
@@ -3344,7 +3344,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>0.40625</v>
       </c>
@@ -3352,7 +3352,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>0.41666666666666702</v>
       </c>
@@ -3360,7 +3360,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>0.42708333333333298</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>0.4375</v>
       </c>
@@ -3376,7 +3376,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>0.44791666666666702</v>
       </c>
@@ -3384,7 +3384,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>0.45833333333333298</v>
       </c>
@@ -3392,7 +3392,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>0.46875</v>
       </c>
@@ -3400,7 +3400,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>0.47916666666666702</v>
       </c>
@@ -3408,7 +3408,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>0.48958333333333298</v>
       </c>
@@ -3416,35 +3416,35 @@
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="73">
         <v>0.5</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="76"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="76"/>
-    </row>
-    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="76"/>
-    </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="72"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="76"/>
-    </row>
-    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="59"/>
+      <c r="D18" s="79"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="74"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="79"/>
+    </row>
+    <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="74"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="79"/>
+    </row>
+    <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="75"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="79"/>
+    </row>
+    <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>0.54166666666666696</v>
       </c>
@@ -3452,7 +3452,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>0.55208333333333304</v>
       </c>
@@ -3460,7 +3460,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>0.5625</v>
       </c>
@@ -3468,7 +3468,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>0.57291666666666696</v>
       </c>
@@ -3476,7 +3476,7 @@
       <c r="C25" s="5"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>0.58333333333333304</v>
       </c>
@@ -3484,7 +3484,7 @@
       <c r="C26" s="5"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>0.59375</v>
       </c>
@@ -3492,7 +3492,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="19">
         <v>0.60416666666666696</v>
       </c>
@@ -3500,15 +3500,15 @@
       <c r="C28" s="5"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>